<commit_message>
w2d2 exercise working but sort of hard coded
</commit_message>
<xml_diff>
--- a/week_2/spreadsheets/inventory.xlsx
+++ b/week_2/spreadsheets/inventory.xlsx
@@ -473,6 +473,11 @@
       <c r="E2" t="n">
         <v>743</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Skip reorder</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -494,6 +499,11 @@
       <c r="E3" t="n">
         <v>101</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Skip reorder</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -515,6 +525,11 @@
       <c r="E4" t="n">
         <v>137</v>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Skip reorder</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -536,6 +551,9 @@
       <c r="E5" t="n">
         <v>364</v>
       </c>
+      <c r="F5" t="n">
+        <v>1136</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -557,6 +575,9 @@
       <c r="E6" t="n">
         <v>120</v>
       </c>
+      <c r="F6" t="n">
+        <v>1880</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -578,6 +599,11 @@
       <c r="E7" t="n">
         <v>85</v>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Skip reorder</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -599,6 +625,9 @@
       <c r="E8" t="n">
         <v>24</v>
       </c>
+      <c r="F8" t="n">
+        <v>176</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -620,6 +649,9 @@
       <c r="E9" t="n">
         <v>12</v>
       </c>
+      <c r="F9" t="n">
+        <v>188</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -641,6 +673,11 @@
       <c r="E10" t="n">
         <v>39</v>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Skip reorder</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -662,6 +699,11 @@
       <c r="E11" t="n">
         <v>234</v>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Skip reorder</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -683,6 +725,11 @@
       <c r="E12" t="n">
         <v>1232</v>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Skip reorder</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -704,6 +751,11 @@
       <c r="E13" t="n">
         <v>11</v>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Skip reorder</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -724,6 +776,9 @@
       </c>
       <c r="E14" t="n">
         <v>249</v>
+      </c>
+      <c r="F14" t="n">
+        <v>751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>